<commit_message>
first working led bar function
</commit_message>
<xml_diff>
--- a/Firmware/Other/shift register layout.xlsx
+++ b/Firmware/Other/shift register layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69f5ad8fb782b24f/Documents/GitHub/Home-Audio-System/Firmware/Other/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indesignllc1-my.sharepoint.com/personal/adwolfe_indesign-llc_com/Documents/M_Drive/Github/Home-Audio-System/Firmware/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{9E05FF3F-3F67-4A25-BEE8-489DB55CCE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B499109-2C22-4D3A-8FCB-4440CE9A8557}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="114_{6763136E-AE71-48F1-96C9-E5D8286F65EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7608C844-FF05-42A2-8EBF-164E95706735}"/>
   <bookViews>
-    <workbookView xWindow="19605" yWindow="4080" windowWidth="15420" windowHeight="15345" xr2:uid="{5C0466F7-E910-47D1-BF49-48D73307B221}"/>
+    <workbookView xWindow="15285" yWindow="0" windowWidth="13620" windowHeight="15585" xr2:uid="{5C0466F7-E910-47D1-BF49-48D73307B221}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>63Hz</t>
   </si>
@@ -63,6 +63,30 @@
   </si>
   <si>
     <t>7 segment</t>
+  </si>
+  <si>
+    <t>want to control 400Hz bar graph</t>
+  </si>
+  <si>
+    <t>first bit is bit number 20</t>
+  </si>
+  <si>
+    <t>home_byte is 2</t>
+  </si>
+  <si>
+    <t>offset_bits is 4</t>
+  </si>
+  <si>
+    <t>assume amplitude of 10</t>
+  </si>
+  <si>
+    <t>need to shift 0xFF left by offset_bits, and OR in with home byte</t>
+  </si>
+  <si>
+    <t>msb</t>
+  </si>
+  <si>
+    <t>lsb</t>
   </si>
 </sst>
 </file>
@@ -86,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -94,15 +118,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,10 +201,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806BADEE-A314-4E44-ABEA-632AB19052C6}">
-  <dimension ref="A1:CR3"/>
+  <dimension ref="A1:CR19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CK3" sqref="CK3:CR3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,405 +535,405 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
       <c r="U1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="3"/>
       <c r="AE1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="3"/>
       <c r="AO1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="3"/>
       <c r="AY1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="1"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="3"/>
       <c r="BI1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BJ1" s="1"/>
-      <c r="BK1" s="1"/>
-      <c r="BL1" s="1"/>
-      <c r="BM1" s="1"/>
-      <c r="BN1" s="1"/>
-      <c r="BO1" s="1"/>
-      <c r="BP1" s="1"/>
-      <c r="BQ1" s="1"/>
-      <c r="BR1" s="1"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="3"/>
       <c r="BS1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="BT1" s="1"/>
-      <c r="BU1" s="1"/>
-      <c r="BV1" s="1"/>
-      <c r="BW1" s="1"/>
-      <c r="BX1" s="1"/>
-      <c r="BY1" s="1"/>
-      <c r="BZ1" s="1"/>
-      <c r="CA1" s="1"/>
-      <c r="CB1" s="1"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+      <c r="CB1" s="3"/>
       <c r="CC1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="CD1" s="1"/>
-      <c r="CE1" s="1"/>
-      <c r="CF1" s="1"/>
-      <c r="CG1" s="1"/>
-      <c r="CH1" s="1"/>
-      <c r="CI1" s="1"/>
-      <c r="CJ1" s="1"/>
-      <c r="CK1" s="1"/>
-      <c r="CL1" s="1"/>
+      <c r="CD1" s="2"/>
+      <c r="CE1" s="2"/>
+      <c r="CF1" s="2"/>
+      <c r="CG1" s="2"/>
+      <c r="CH1" s="2"/>
+      <c r="CI1" s="2"/>
+      <c r="CJ1" s="2"/>
+      <c r="CK1" s="2"/>
+      <c r="CL1" s="3"/>
       <c r="CM1" s="1"/>
-      <c r="CN1" s="1"/>
-      <c r="CO1" s="1"/>
-      <c r="CP1" s="1"/>
-      <c r="CQ1" s="1"/>
-      <c r="CR1" s="1"/>
+      <c r="CN1" s="2"/>
+      <c r="CO1" s="2"/>
+      <c r="CP1" s="2"/>
+      <c r="CQ1" s="2"/>
+      <c r="CR1" s="2"/>
     </row>
     <row r="2" spans="1:96" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>11</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>13</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>15</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="4">
         <v>16</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="4">
         <v>17</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="4">
         <v>18</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="4">
         <v>19</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="4">
         <v>20</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="4">
         <v>21</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="4">
         <v>22</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="4">
         <v>23</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="4">
         <v>24</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="4">
         <v>25</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="4">
         <v>26</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="4">
         <v>27</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="4">
         <v>28</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="4">
         <v>29</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="4">
         <v>30</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="4">
         <v>31</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="4">
         <v>32</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="4">
         <v>33</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="4">
         <v>34</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="4">
         <v>35</v>
       </c>
-      <c r="AK2">
+      <c r="AK2" s="4">
         <v>36</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="4">
         <v>37</v>
       </c>
-      <c r="AM2">
+      <c r="AM2" s="4">
         <v>38</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="4">
         <v>39</v>
       </c>
-      <c r="AO2">
+      <c r="AO2" s="4">
         <v>40</v>
       </c>
-      <c r="AP2">
+      <c r="AP2" s="4">
         <v>41</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ2" s="4">
         <v>42</v>
       </c>
-      <c r="AR2">
+      <c r="AR2" s="4">
         <v>43</v>
       </c>
-      <c r="AS2">
+      <c r="AS2" s="4">
         <v>44</v>
       </c>
-      <c r="AT2">
+      <c r="AT2" s="4">
         <v>45</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="4">
         <v>46</v>
       </c>
-      <c r="AV2">
+      <c r="AV2" s="4">
         <v>47</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="4">
         <v>48</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="4">
         <v>49</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" s="4">
         <v>50</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="4">
         <v>51</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="4">
         <v>52</v>
       </c>
-      <c r="BB2">
+      <c r="BB2" s="4">
         <v>53</v>
       </c>
-      <c r="BC2">
+      <c r="BC2" s="4">
         <v>54</v>
       </c>
-      <c r="BD2">
+      <c r="BD2" s="4">
         <v>55</v>
       </c>
-      <c r="BE2">
+      <c r="BE2" s="4">
         <v>56</v>
       </c>
-      <c r="BF2">
+      <c r="BF2" s="4">
         <v>57</v>
       </c>
-      <c r="BG2">
+      <c r="BG2" s="4">
         <v>58</v>
       </c>
-      <c r="BH2">
+      <c r="BH2" s="4">
         <v>59</v>
       </c>
-      <c r="BI2">
+      <c r="BI2" s="4">
         <v>60</v>
       </c>
-      <c r="BJ2">
+      <c r="BJ2" s="4">
         <v>61</v>
       </c>
-      <c r="BK2">
+      <c r="BK2" s="4">
         <v>62</v>
       </c>
-      <c r="BL2">
+      <c r="BL2" s="4">
         <v>63</v>
       </c>
-      <c r="BM2">
+      <c r="BM2" s="4">
         <v>64</v>
       </c>
-      <c r="BN2">
+      <c r="BN2" s="4">
         <v>65</v>
       </c>
-      <c r="BO2">
+      <c r="BO2" s="4">
         <v>66</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="4">
         <v>67</v>
       </c>
-      <c r="BQ2">
+      <c r="BQ2" s="4">
         <v>68</v>
       </c>
-      <c r="BR2">
+      <c r="BR2" s="4">
         <v>69</v>
       </c>
-      <c r="BS2">
+      <c r="BS2" s="4">
         <v>70</v>
       </c>
-      <c r="BT2">
+      <c r="BT2" s="4">
         <v>71</v>
       </c>
-      <c r="BU2">
+      <c r="BU2" s="4">
         <v>72</v>
       </c>
-      <c r="BV2">
+      <c r="BV2" s="4">
         <v>73</v>
       </c>
-      <c r="BW2">
+      <c r="BW2" s="4">
         <v>74</v>
       </c>
-      <c r="BX2">
+      <c r="BX2" s="4">
         <v>75</v>
       </c>
-      <c r="BY2">
+      <c r="BY2" s="4">
         <v>76</v>
       </c>
-      <c r="BZ2">
+      <c r="BZ2" s="4">
         <v>77</v>
       </c>
-      <c r="CA2">
+      <c r="CA2" s="4">
         <v>78</v>
       </c>
-      <c r="CB2">
+      <c r="CB2" s="4">
         <v>79</v>
       </c>
-      <c r="CC2">
+      <c r="CC2" s="4">
         <v>80</v>
       </c>
-      <c r="CD2">
+      <c r="CD2" s="4">
         <v>81</v>
       </c>
-      <c r="CE2">
+      <c r="CE2" s="4">
         <v>82</v>
       </c>
-      <c r="CF2">
+      <c r="CF2" s="4">
         <v>83</v>
       </c>
-      <c r="CG2">
+      <c r="CG2" s="4">
         <v>84</v>
       </c>
-      <c r="CH2">
+      <c r="CH2" s="4">
         <v>85</v>
       </c>
-      <c r="CI2">
+      <c r="CI2" s="4">
         <v>86</v>
       </c>
-      <c r="CJ2">
+      <c r="CJ2" s="4">
         <v>87</v>
       </c>
-      <c r="CK2">
+      <c r="CK2" s="4">
         <v>88</v>
       </c>
-      <c r="CL2">
+      <c r="CL2" s="4">
         <v>89</v>
       </c>
-      <c r="CM2">
+      <c r="CM2" s="4">
         <v>90</v>
       </c>
-      <c r="CN2">
+      <c r="CN2" s="4">
         <v>91</v>
       </c>
-      <c r="CO2">
+      <c r="CO2" s="4">
         <v>92</v>
       </c>
-      <c r="CP2">
+      <c r="CP2" s="4">
         <v>93</v>
       </c>
-      <c r="CQ2">
+      <c r="CQ2" s="4">
         <v>94</v>
       </c>
-      <c r="CR2">
+      <c r="CR2" s="4">
         <v>95</v>
       </c>
     </row>
@@ -862,133 +941,170 @@
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="3"/>
       <c r="Q3" s="1">
         <v>2</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="3"/>
       <c r="Y3" s="1">
         <v>3</v>
       </c>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="3"/>
       <c r="AG3" s="1">
         <v>4</v>
       </c>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="3"/>
       <c r="AO3" s="1">
         <v>5</v>
       </c>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-      <c r="AV3" s="1"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="3"/>
       <c r="AW3" s="1">
         <v>6</v>
       </c>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
-      <c r="AZ3" s="1"/>
-      <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="3"/>
       <c r="BE3" s="1">
         <v>7</v>
       </c>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="BI3" s="1"/>
-      <c r="BJ3" s="1"/>
-      <c r="BK3" s="1"/>
-      <c r="BL3" s="1"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="3"/>
       <c r="BM3" s="1">
         <v>8</v>
       </c>
-      <c r="BN3" s="1"/>
-      <c r="BO3" s="1"/>
-      <c r="BP3" s="1"/>
-      <c r="BQ3" s="1"/>
-      <c r="BR3" s="1"/>
-      <c r="BS3" s="1"/>
-      <c r="BT3" s="1"/>
+      <c r="BN3" s="2"/>
+      <c r="BO3" s="2"/>
+      <c r="BP3" s="2"/>
+      <c r="BQ3" s="2"/>
+      <c r="BR3" s="2"/>
+      <c r="BS3" s="2"/>
+      <c r="BT3" s="3"/>
       <c r="BU3" s="1">
         <v>9</v>
       </c>
-      <c r="BV3" s="1"/>
-      <c r="BW3" s="1"/>
-      <c r="BX3" s="1"/>
-      <c r="BY3" s="1"/>
-      <c r="BZ3" s="1"/>
-      <c r="CA3" s="1"/>
-      <c r="CB3" s="1"/>
+      <c r="BV3" s="2"/>
+      <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
+      <c r="BY3" s="2"/>
+      <c r="BZ3" s="2"/>
+      <c r="CA3" s="2"/>
+      <c r="CB3" s="3"/>
       <c r="CC3" s="1">
         <v>10</v>
       </c>
-      <c r="CD3" s="1"/>
-      <c r="CE3" s="1"/>
-      <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
-      <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
+      <c r="CD3" s="2"/>
+      <c r="CE3" s="2"/>
+      <c r="CF3" s="2"/>
+      <c r="CG3" s="2"/>
+      <c r="CH3" s="2"/>
+      <c r="CI3" s="2"/>
+      <c r="CJ3" s="3"/>
       <c r="CK3" s="1">
         <v>11</v>
       </c>
-      <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
-      <c r="CN3" s="1"/>
-      <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
-      <c r="CR3" s="1"/>
+      <c r="CL3" s="2"/>
+      <c r="CM3" s="2"/>
+      <c r="CN3" s="2"/>
+      <c r="CO3" s="2"/>
+      <c r="CP3" s="2"/>
+      <c r="CQ3" s="2"/>
+      <c r="CR3" s="3"/>
+    </row>
+    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="CC3:CJ3"/>
-    <mergeCell ref="CK3:CR3"/>
-    <mergeCell ref="AO3:AV3"/>
-    <mergeCell ref="AW3:BD3"/>
-    <mergeCell ref="BE3:BL3"/>
-    <mergeCell ref="BM3:BT3"/>
-    <mergeCell ref="BU3:CB3"/>
+  <mergeCells count="22">
+    <mergeCell ref="CC1:CL1"/>
+    <mergeCell ref="CM1:CR1"/>
+    <mergeCell ref="AO1:AX1"/>
+    <mergeCell ref="AY1:BH1"/>
+    <mergeCell ref="BI1:BR1"/>
+    <mergeCell ref="BS1:CB1"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="U1:AD1"/>
@@ -998,11 +1114,13 @@
     <mergeCell ref="Q3:X3"/>
     <mergeCell ref="Y3:AF3"/>
     <mergeCell ref="AG3:AN3"/>
-    <mergeCell ref="AO1:AX1"/>
-    <mergeCell ref="AY1:BH1"/>
-    <mergeCell ref="BI1:BR1"/>
-    <mergeCell ref="BS1:CB1"/>
-    <mergeCell ref="CC1:CR1"/>
+    <mergeCell ref="CC3:CJ3"/>
+    <mergeCell ref="CK3:CR3"/>
+    <mergeCell ref="AO3:AV3"/>
+    <mergeCell ref="AW3:BD3"/>
+    <mergeCell ref="BE3:BL3"/>
+    <mergeCell ref="BM3:BT3"/>
+    <mergeCell ref="BU3:CB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>